<commit_message>
daile stone in transaction updates
dsi
- dsi insert
- stock updates
</commit_message>
<xml_diff>
--- a/designs/tables with sample data.xlsx
+++ b/designs/tables with sample data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="11415" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15165" windowHeight="4425"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,77 +12,17 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Kiran Yadav</author>
-  </authors>
-  <commentList>
-    <comment ref="D6" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Kiran Yadav:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-SMS: DSI:[A+,5],[A,10],[A-,1]</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I6" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Kiran Yadav:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-only one entry always for each range</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>in date</t>
   </si>
   <si>
     <t>range</t>
-  </si>
-  <si>
-    <t>stone in</t>
   </si>
   <si>
     <t>comments</t>
@@ -111,32 +51,28 @@
   </si>
   <si>
     <t>powder produced</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>qulity_range_id</t>
+  </si>
+  <si>
+    <t>stone in qty</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -171,10 +107,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -470,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D6:K21"/>
+  <dimension ref="C6:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -482,46 +418,52 @@
     <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.140625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="24.140625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="4:11">
-      <c r="D6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="I6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="4:11">
+    <row r="6" spans="3:11">
+      <c r="D6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="I6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="3:11">
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="I7" t="s">
         <v>3</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="K7" t="s">
         <v>5</v>
       </c>
-      <c r="K7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="4:11" ht="105">
+    </row>
+    <row r="8" spans="3:11" ht="105">
+      <c r="C8">
+        <v>1</v>
+      </c>
       <c r="D8" s="3">
         <v>42865</v>
       </c>
@@ -535,11 +477,14 @@
       <c r="I8">
         <v>1</v>
       </c>
-      <c r="J8" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="4:11">
+      <c r="J8" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11">
+      <c r="C9">
+        <v>1</v>
+      </c>
       <c r="D9" s="3">
         <v>42865</v>
       </c>
@@ -554,7 +499,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="4:11">
+    <row r="10" spans="3:11">
+      <c r="C10">
+        <v>1</v>
+      </c>
       <c r="D10" s="3">
         <v>42865</v>
       </c>
@@ -569,7 +517,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="4:11">
+    <row r="11" spans="3:11">
+      <c r="C11">
+        <v>1</v>
+      </c>
       <c r="D11" s="3">
         <v>42865</v>
       </c>
@@ -584,7 +535,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="4:11">
+    <row r="12" spans="3:11">
+      <c r="C12">
+        <v>1</v>
+      </c>
       <c r="D12" s="3">
         <v>42865</v>
       </c>
@@ -599,21 +553,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="4:11">
+    <row r="16" spans="3:11">
       <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
         <v>9</v>
       </c>
-      <c r="E16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>10</v>
       </c>
-      <c r="G16" t="s">
-        <v>11</v>
-      </c>
       <c r="H16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="4:6">
@@ -677,7 +631,6 @@
     <mergeCell ref="I6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>